<commit_message>
[ANV] updated silicon and xenon spreadsheets
</commit_message>
<xml_diff>
--- a/levelfiles/spreadsheet/silicon.xlsx
+++ b/levelfiles/spreadsheet/silicon.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/villaa/Computing/nrCascadeSim/levelfiles/spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA7B523D-803B-7643-91D7-CB2A7CEAA709}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12D21A97-B536-E541-804C-3C86B46079A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="1560" windowWidth="28040" windowHeight="17040" activeTab="3" xr2:uid="{2D1C8EBD-58BF-0748-ACC6-F1ED1991D975}"/>
+    <workbookView xWindow="380" yWindow="1560" windowWidth="28040" windowHeight="17040" activeTab="1" xr2:uid="{2D1C8EBD-58BF-0748-ACC6-F1ED1991D975}"/>
   </bookViews>
   <sheets>
     <sheet name="isotopes" sheetId="1" r:id="rId1"/>
@@ -605,7 +605,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80AAE235-F126-8A49-B3BB-0FA674935FB4}">
   <dimension ref="A1:G102"/>
   <sheetViews>
-    <sheetView topLeftCell="A92" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A102" sqref="A102:XFD102"/>
     </sheetView>
   </sheetViews>
@@ -1578,7 +1578,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDB23933-7A95-2343-B99C-FDD641BDEE2A}">
   <dimension ref="A1:G154"/>
   <sheetViews>
-    <sheetView topLeftCell="A135" workbookViewId="0">
+    <sheetView topLeftCell="A126" workbookViewId="0">
       <selection activeCell="A154" sqref="A154:XFD154"/>
     </sheetView>
   </sheetViews>
@@ -3010,7 +3010,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5D52D8F-C47E-B24E-A2B9-BD42B304AD19}">
   <dimension ref="A1:G118"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>

</xml_diff>